<commit_message>
Started IO sheet and finished calculator spreadsheet
Started an IO sheet for all signals on PDB. Need to assign IO to Arduino and add various power and ground signals for terminal blocks.
</commit_message>
<xml_diff>
--- a/Functional Requirements/Tables/Power Distribution Board Component Selection.xlsx
+++ b/Functional Requirements/Tables/Power Distribution Board Component Selection.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Vertical Garden\Schematic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\Dionysus-PowerDistributionBoard\Functional Requirements\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BE82F-A73D-44A2-8124-3C7ABEDEFD8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D746C2C-4E8D-4FCE-9D6C-62E19699F062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{03132853-3FF9-4576-9F22-D609AA62A077}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{03132853-3FF9-4576-9F22-D609AA62A077}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="12" r:id="rId1"/>
-    <sheet name="Terminal Block" sheetId="4" r:id="rId2"/>
-    <sheet name="LED" sheetId="7" r:id="rId3"/>
-    <sheet name="Misc. Functions" sheetId="11" r:id="rId4"/>
-    <sheet name="Alternative Parts List" sheetId="8" r:id="rId5"/>
-    <sheet name="Power Consumption" sheetId="5" r:id="rId6"/>
-    <sheet name="Sheet 1" sheetId="9" r:id="rId7"/>
+    <sheet name="Terminal Block (2)" sheetId="13" r:id="rId2"/>
+    <sheet name="Terminal Block" sheetId="4" r:id="rId3"/>
+    <sheet name="LED" sheetId="7" r:id="rId4"/>
+    <sheet name="Misc. Functions" sheetId="11" r:id="rId5"/>
+    <sheet name="Alternative Parts List" sheetId="8" r:id="rId6"/>
+    <sheet name="Power Consumption" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet 1" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="258">
   <si>
     <t>I2C termination jumpers</t>
   </si>
@@ -592,6 +593,219 @@
   </si>
   <si>
     <t>Signal (0-5V)</t>
+  </si>
+  <si>
+    <t>1-WIRE</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>USART</t>
+  </si>
+  <si>
+    <t>TWI-2</t>
+  </si>
+  <si>
+    <t>TWI-1</t>
+  </si>
+  <si>
+    <t>GPIO (ANALOG)</t>
+  </si>
+  <si>
+    <t>GPIO (DIGITAL)</t>
+  </si>
+  <si>
+    <t>EZO SENSOR 4</t>
+  </si>
+  <si>
+    <t>EZO SENSOR 3</t>
+  </si>
+  <si>
+    <t>EZO SENSOR 2</t>
+  </si>
+  <si>
+    <t>EZO SENSOR 1</t>
+  </si>
+  <si>
+    <t>TEMP SENSOR 5</t>
+  </si>
+  <si>
+    <t>TEMP SENSOR 4</t>
+  </si>
+  <si>
+    <t>TEMP SENSOR 3</t>
+  </si>
+  <si>
+    <t>TEMP SENSOR 2</t>
+  </si>
+  <si>
+    <t>TEMP SENSOR 1</t>
+  </si>
+  <si>
+    <t>AMB ENVIRONMENT</t>
+  </si>
+  <si>
+    <t>RSVR LVL MIN</t>
+  </si>
+  <si>
+    <t>RSVR LVL MED</t>
+  </si>
+  <si>
+    <t>RSVR LVL MAX</t>
+  </si>
+  <si>
+    <t>E-STOP</t>
+  </si>
+  <si>
+    <t>AMBIENT LIGHT SENSOR</t>
+  </si>
+  <si>
+    <t>RESERVOIR HEATER</t>
+  </si>
+  <si>
+    <t>RESERVOIR PUMP</t>
+  </si>
+  <si>
+    <t>CHEM 5 LEVEL MIN</t>
+  </si>
+  <si>
+    <t>CHEM 4 LEVEL MIN</t>
+  </si>
+  <si>
+    <t>CHEM 3 LEVEL MIN</t>
+  </si>
+  <si>
+    <t>CHEM 2 LEVEL MIN</t>
+  </si>
+  <si>
+    <t>CHEM 1 LEVEL MIN</t>
+  </si>
+  <si>
+    <t>NCS PUMP</t>
+  </si>
+  <si>
+    <t>PER PUMP 5 PWR</t>
+  </si>
+  <si>
+    <t>PER PUMP 4 PWR</t>
+  </si>
+  <si>
+    <t>PER PUMP 3 PWR</t>
+  </si>
+  <si>
+    <t>PER PUMP 2 PWR</t>
+  </si>
+  <si>
+    <t>PER PUMP 1 PWR</t>
+  </si>
+  <si>
+    <t>LED CH8</t>
+  </si>
+  <si>
+    <t>LED CH7</t>
+  </si>
+  <si>
+    <t>LED CH6</t>
+  </si>
+  <si>
+    <t>LED CH5</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/phoenix-contact/1929517/638167</t>
+  </si>
+  <si>
+    <t>LED CH4</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/phoenix-contact/1715022/260626</t>
+  </si>
+  <si>
+    <t>LED CH3</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/wago-corporation/2604-3102/15528152</t>
+  </si>
+  <si>
+    <t>LED CH2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/filter/terminal-blocks-wire-to-board/371?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIAzAExhgCsALCIQ7QBxwDszIrYcYNjz4CELWnCowQAXUIAHAC5QQAZUUAnAJYA7AOYgAvoTYAGKohApIGHAWJlKdGGAYXxcRgjkglK9dr6RoRgppx0lta2eIQkkORg8FSesgrKkGqaugbG4Axs3NBWaFgxDvG8pqYwdBEsVTXS9dV0Qs01Fj5%2BGQHZweBwHJEldrGOpqm%2B6ZmBOYQ0tcM2pfZx5LUABACCPHSc27tsB4QuxyA1ZzAwZ6FgB13TAKo6WooA8qgAsrjo2ACuGlw-RoMCERSiKzGFQgDxUAEkdIpcHpcBojLkIkV5FAwApsZAqHRctIiloACYqAC0oXcUxUPEUAE95ECMmTsChDIYgA</t>
+  </si>
+  <si>
+    <t>LED CH1</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>Current [A]</t>
+  </si>
+  <si>
+    <t>Voltage [V]</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Vertical with Board</t>
+  </si>
+  <si>
+    <t>Screwless or Screw</t>
+  </si>
+  <si>
+    <t>Through Hole</t>
+  </si>
+  <si>
+    <t>&gt;24</t>
+  </si>
+  <si>
+    <t>15 to 60</t>
+  </si>
+  <si>
+    <t>Horizontal with Board</t>
+  </si>
+  <si>
+    <t>2 through 10</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Wire Termination</t>
+  </si>
+  <si>
+    <t>Mounting Type</t>
+  </si>
+  <si>
+    <t>Wire Gauge</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Mating Orientation</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>Positions Per Level</t>
+  </si>
+  <si>
+    <t>Number of Levels</t>
+  </si>
+  <si>
+    <t>Component Filter Parameters</t>
   </si>
 </sst>
 </file>
@@ -601,7 +815,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +834,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -924,11 +1146,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1018,12 +1241,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1055,9 +1272,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1372,16 +1600,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC225F3-62B8-4465-89CF-7FA332C742CA}">
   <dimension ref="B2:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>152</v>
       </c>
@@ -1389,12 +1617,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>153</v>
       </c>
@@ -1402,22 +1630,22 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>161</v>
       </c>
@@ -1425,7 +1653,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>158</v>
       </c>
@@ -1433,27 +1661,27 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>154</v>
       </c>
@@ -1461,17 +1689,17 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>155</v>
       </c>
@@ -1479,7 +1707,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>156</v>
       </c>
@@ -1487,25 +1715,25 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>157</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="41" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="43" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="41" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -1513,17 +1741,17 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>159</v>
       </c>
@@ -1531,12 +1759,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>160</v>
       </c>
@@ -1544,12 +1772,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>184</v>
       </c>
@@ -1560,6 +1788,757 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF0081B-92FF-4470-A1DB-880DCDD20CE9}">
+  <dimension ref="A1:L60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="L18" s="44" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>231</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="L19" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>17</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="L20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>17</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="L21" s="44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3</v>
+      </c>
+      <c r="G24" s="1">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>222</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>17</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>221</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>24</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>220</v>
+      </c>
+      <c r="F27" s="1">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>24</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>219</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>24</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>24</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>24</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>216</v>
+      </c>
+      <c r="F31" s="1">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <v>32</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3</v>
+      </c>
+      <c r="G32" s="1">
+        <v>16</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3</v>
+      </c>
+      <c r="G33" s="1">
+        <v>16</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>213</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3</v>
+      </c>
+      <c r="G34" s="1">
+        <v>16</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
+      <c r="G35" s="1">
+        <v>16</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="1">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1">
+        <v>16</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>210</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>32</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>209</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
+      <c r="G38" s="1">
+        <v>32</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>208</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="G39" s="1">
+        <v>12</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>207</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+      <c r="G40" s="1">
+        <v>24</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3</v>
+      </c>
+      <c r="G41" s="1">
+        <v>16</v>
+      </c>
+      <c r="H41" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>205</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3</v>
+      </c>
+      <c r="G42" s="1">
+        <v>16</v>
+      </c>
+      <c r="H42" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>204</v>
+      </c>
+      <c r="F43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1">
+        <v>16</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>203</v>
+      </c>
+      <c r="F44" s="1">
+        <v>4</v>
+      </c>
+      <c r="G44" s="1">
+        <v>5</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>202</v>
+      </c>
+      <c r="F45" s="1">
+        <v>3</v>
+      </c>
+      <c r="G45" s="1">
+        <v>5</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>201</v>
+      </c>
+      <c r="F46" s="1">
+        <v>3</v>
+      </c>
+      <c r="G46" s="1">
+        <v>5</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="1">
+        <v>3</v>
+      </c>
+      <c r="G47" s="1">
+        <v>5</v>
+      </c>
+      <c r="H47" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>199</v>
+      </c>
+      <c r="F48" s="1">
+        <v>3</v>
+      </c>
+      <c r="G48" s="1">
+        <v>5</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>198</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3</v>
+      </c>
+      <c r="G49" s="1">
+        <v>5</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>197</v>
+      </c>
+      <c r="F50" s="1">
+        <v>3</v>
+      </c>
+      <c r="G50" s="1">
+        <v>5</v>
+      </c>
+      <c r="H50" s="1">
+        <f>20/1000</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>196</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3</v>
+      </c>
+      <c r="G51" s="1">
+        <v>5</v>
+      </c>
+      <c r="H51" s="1">
+        <f>20/1000</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>195</v>
+      </c>
+      <c r="F52" s="1">
+        <v>3</v>
+      </c>
+      <c r="G52" s="1">
+        <v>5</v>
+      </c>
+      <c r="H52" s="1">
+        <f>20/1000</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>194</v>
+      </c>
+      <c r="F53" s="1">
+        <v>3</v>
+      </c>
+      <c r="G53" s="1">
+        <v>5</v>
+      </c>
+      <c r="H53" s="1">
+        <f>20/1000</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>193</v>
+      </c>
+      <c r="F54" s="1">
+        <v>12</v>
+      </c>
+      <c r="G54" s="1">
+        <v>3</v>
+      </c>
+      <c r="H54" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>192</v>
+      </c>
+      <c r="F55" s="1">
+        <v>7</v>
+      </c>
+      <c r="G55" s="1">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>191</v>
+      </c>
+      <c r="F56" s="1">
+        <v>4</v>
+      </c>
+      <c r="G56" s="1">
+        <v>3</v>
+      </c>
+      <c r="H56" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>190</v>
+      </c>
+      <c r="F57" s="1">
+        <v>4</v>
+      </c>
+      <c r="G57" s="1">
+        <v>3</v>
+      </c>
+      <c r="H57" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>189</v>
+      </c>
+      <c r="F58" s="1">
+        <v>4</v>
+      </c>
+      <c r="G58" s="1">
+        <v>3</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F59" s="1">
+        <v>4</v>
+      </c>
+      <c r="G59" s="1">
+        <v>3</v>
+      </c>
+      <c r="H59" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>187</v>
+      </c>
+      <c r="F60" s="1">
+        <v>3</v>
+      </c>
+      <c r="G60" s="1">
+        <v>3</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L21" r:id="rId1" xr:uid="{6142C350-45AF-49F0-A060-993E609CDFAF}"/>
+    <hyperlink ref="L18" r:id="rId2" display="https://www.digikey.com/en/products/filter/terminal-blocks-wire-to-board/371?s=N4IgjCBcoGwJxVAYygMwIYBsDOBTANCAPZQDaIAzAExhgCsALCIQ7QBxwDszIrYcYNjz4CELWnCowQAXUIAHAC5QQAZUUAnAJYA7AOYgAvoTYAGKohApIGHAWJlKdGGAYXxcRgjkglK9dr6RoRgppx0lta2eIQkkORg8FSesgrKkGqaugbG4Axs3NBWaFgxDvG8pqYwdBEsVTXS9dV0Qs01Fj5%2BGQHZweBwHJEldrGOpqm%2B6ZmBOYQ0tcM2pfZx5LUABACCPHSc27tsB4QuxyA1ZzAwZ6FgB13TAKo6WooA8qgAsrjo2ACuGlw-RoMCERSiKzGFQgDxUAEkdIpcHpcBojLkIkV5FAwApsZAqHRctIiloACYqAC0oXcUxUPEUAE95ECMmTsChDIYgA" xr:uid="{B91BCCD3-E1F4-45B8-A6C5-E40AB8BD8856}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386FB538-AC50-4DD8-A008-0867B26F7CBE}">
   <dimension ref="B1:K9"/>
   <sheetViews>
@@ -1567,24 +2546,24 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="30.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
@@ -1597,13 +2576,13 @@
       <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="31" t="s">
         <v>135</v>
       </c>
       <c r="I2" s="21" t="s">
@@ -1616,39 +2595,39 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="34">
         <v>1733415</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="37">
         <v>300</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="37">
         <v>15</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="34">
         <v>2</v>
       </c>
-      <c r="J3" s="41">
+      <c r="J3" s="39">
         <v>1.41</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="35" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>83</v>
       </c>
@@ -1661,10 +2640,10 @@
       <c r="E4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="38">
         <v>300</v>
       </c>
-      <c r="G4" s="40">
+      <c r="G4" s="38">
         <v>15</v>
       </c>
       <c r="H4" s="7" t="s">
@@ -1673,14 +2652,14 @@
       <c r="I4" s="6">
         <v>5</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="40">
         <v>1.41</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>82</v>
       </c>
@@ -1693,10 +2672,10 @@
       <c r="E5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="40">
+      <c r="F5" s="38">
         <v>300</v>
       </c>
-      <c r="G5" s="40">
+      <c r="G5" s="38">
         <v>15</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -1705,14 +2684,14 @@
       <c r="I5" s="6">
         <v>3</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="40">
         <v>1.41</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="K5" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>138</v>
       </c>
@@ -1725,10 +2704,10 @@
       <c r="E6" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="38">
         <v>250</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="38">
         <v>24</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -1737,14 +2716,14 @@
       <c r="I6" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="40">
         <v>20.5</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="36" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>141</v>
       </c>
@@ -1757,10 +2736,10 @@
       <c r="E7" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="38">
         <v>600</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="38">
         <v>60</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -1769,14 +2748,14 @@
       <c r="I7" s="6">
         <v>2</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="40">
         <v>11.08</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="36" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>144</v>
       </c>
@@ -1789,10 +2768,10 @@
       <c r="E8" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="38">
         <v>300</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="38">
         <v>10</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1801,14 +2780,14 @@
       <c r="I8" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="40">
         <v>1.23</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>150</v>
       </c>
@@ -1821,10 +2800,10 @@
       <c r="E9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="38">
         <v>150</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="38">
         <v>6</v>
       </c>
       <c r="H9" s="7" t="s">
@@ -1833,10 +2812,10 @@
       <c r="I9" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="40">
         <v>2.59</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="36" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1846,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D1737A-BD25-4E8D-8794-0E0CABF11A04}">
   <dimension ref="B1:H14"/>
   <sheetViews>
@@ -1854,21 +2833,21 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
@@ -1891,7 +2870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>108</v>
       </c>
@@ -1914,7 +2893,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>108</v>
       </c>
@@ -1937,7 +2916,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="13"/>
       <c r="C5" s="9"/>
       <c r="D5" s="8"/>
@@ -1950,7 +2929,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
@@ -1965,7 +2944,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="15"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
@@ -1980,7 +2959,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="15"/>
       <c r="C8" s="7"/>
       <c r="D8" s="6"/>
@@ -1989,7 +2968,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="15"/>
       <c r="C9" s="7"/>
       <c r="D9" s="6"/>
@@ -1998,7 +2977,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="28"/>
     </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
@@ -2007,16 +2986,16 @@
       <c r="G10" s="19"/>
       <c r="H10" s="29"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H13"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H14"/>
     </row>
   </sheetData>
@@ -2025,7 +3004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8CD6C7-D1E8-4AD0-81BB-1B152B222F00}">
   <dimension ref="B1:F18"/>
   <sheetViews>
@@ -2033,19 +3012,19 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3"/>
-    <col min="7" max="16384" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
@@ -2062,103 +3041,103 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25"/>
       <c r="E3" s="24"/>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="15"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="15"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="6"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="30"/>
       <c r="E14" s="7"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="30"/>
       <c r="E15" s="7"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D16"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18"/>
     </row>
   </sheetData>
@@ -2167,7 +3146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0947EE23-9ECF-4592-8F51-749802C34EDA}">
   <dimension ref="B1:F8"/>
   <sheetViews>
@@ -2175,18 +3154,17 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
@@ -2203,7 +3181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>97</v>
       </c>
@@ -2218,7 +3196,7 @@
       </c>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>103</v>
       </c>
@@ -2233,28 +3211,28 @@
       </c>
       <c r="F4" s="16"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="16"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="15"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
       <c r="D8" s="19"/>
@@ -2266,7 +3244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCADC25-0920-42FB-BE76-D952573FE4D3}">
   <dimension ref="B1:S14"/>
   <sheetViews>
@@ -2274,22 +3252,22 @@
       <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="31" t="s">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="C1" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
       <c r="H1" t="s">
         <v>75</v>
       </c>
@@ -2300,7 +3278,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>50</v>
       </c>
@@ -2340,7 +3318,7 @@
         <v>1.159</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>47</v>
       </c>
@@ -2378,7 +3356,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>48</v>
       </c>
@@ -2402,7 +3380,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>49</v>
       </c>
@@ -2426,7 +3404,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>54</v>
       </c>
@@ -2447,7 +3425,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>67</v>
       </c>
@@ -2470,12 +3448,12 @@
         <f>G7*D7</f>
         <v>68.5</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="M7" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="N7" s="31"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N7" s="42"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>68</v>
       </c>
@@ -2505,7 +3483,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -2522,7 +3500,7 @@
         <f>G9*C9</f>
         <v>11.25</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="43" t="s">
         <v>65</v>
       </c>
       <c r="L9" t="s">
@@ -2535,7 +3513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>45</v>
       </c>
@@ -2552,7 +3530,7 @@
         <f>C10*G10</f>
         <v>4.9499999999999993</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="43"/>
       <c r="L10" t="s">
         <v>57</v>
       </c>
@@ -2567,8 +3545,8 @@
         <v>1481.8</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K11" s="32"/>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K11" s="43"/>
       <c r="L11" t="s">
         <v>58</v>
       </c>
@@ -2579,8 +3557,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K12" s="32"/>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K12" s="43"/>
       <c r="L12" t="s">
         <v>59</v>
       </c>
@@ -2591,8 +3569,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K13" s="32"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K13" s="43"/>
       <c r="L13" t="s">
         <v>60</v>
       </c>
@@ -2603,8 +3581,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K14" s="32"/>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K14" s="43"/>
       <c r="L14" t="s">
         <v>61</v>
       </c>
@@ -2626,7 +3604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C23ED62-0ECC-4A44-BB75-01706CEF30B6}">
   <dimension ref="A1:R39"/>
   <sheetViews>
@@ -2634,19 +3612,19 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3"/>
-    <col min="7" max="16384" width="8.85546875" style="2"/>
+    <col min="6" max="6" width="8.88671875" style="3"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:18" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:18" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
@@ -2667,7 +3645,7 @@
       </c>
       <c r="K2"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>82</v>
       </c>
@@ -2688,7 +3666,7 @@
       </c>
       <c r="K3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="15" t="s">
         <v>128</v>
       </c>
@@ -2709,7 +3687,7 @@
       </c>
       <c r="K4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" s="15" t="s">
         <v>77</v>
       </c>
@@ -2730,7 +3708,7 @@
       </c>
       <c r="K5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
@@ -2745,7 +3723,7 @@
       </c>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
@@ -2760,7 +3738,7 @@
       </c>
       <c r="K7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="6"/>
@@ -2771,7 +3749,7 @@
       </c>
       <c r="K8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
@@ -2781,7 +3759,7 @@
       </c>
       <c r="K9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
@@ -2792,7 +3770,7 @@
       </c>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
@@ -2803,7 +3781,7 @@
       </c>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
@@ -2814,7 +3792,7 @@
       </c>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="30"/>
@@ -2825,7 +3803,7 @@
       </c>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="30"/>
@@ -2836,14 +3814,14 @@
       </c>
       <c r="K14"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D15"/>
       <c r="J15" t="s">
         <v>46</v>
       </c>
       <c r="K15"/>
     </row>
-    <row r="16" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="D16"/>
@@ -2863,7 +3841,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
     </row>
-    <row r="17" spans="1:18" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="10" t="s">
         <v>14</v>
@@ -2893,7 +3871,7 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
         <v>77</v>
       </c>
@@ -2912,7 +3890,7 @@
       <c r="J18"/>
       <c r="K18"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>82</v>
       </c>
@@ -2933,7 +3911,7 @@
       </c>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>83</v>
       </c>
@@ -2954,7 +3932,7 @@
       </c>
       <c r="K20"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
         <v>84</v>
       </c>
@@ -2977,7 +3955,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
@@ -2994,7 +3972,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="6"/>
@@ -3011,7 +3989,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
         <v>100</v>
       </c>
@@ -3034,7 +4012,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="7" t="s">
@@ -3046,7 +4024,7 @@
       <c r="J25"/>
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>122</v>
       </c>
@@ -3067,7 +4045,7 @@
       </c>
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>108</v>
       </c>
@@ -3090,7 +4068,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="6"/>
@@ -3105,7 +4083,7 @@
       </c>
       <c r="K28"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="30"/>
@@ -3116,7 +4094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="30"/>
@@ -3127,8 +4105,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10" t="s">
         <v>14</v>
       </c>
@@ -3145,7 +4123,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="13" t="s">
         <v>21</v>
       </c>
@@ -3162,7 +4140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="s">
         <v>24</v>
       </c>
@@ -3179,7 +4157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="15" t="s">
         <v>27</v>
       </c>
@@ -3196,7 +4174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
         <v>33</v>
       </c>
@@ -3213,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
         <v>38</v>
       </c>
@@ -3230,7 +4208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="17" t="s">
         <v>31</v>
       </c>

</xml_diff>